<commit_message>
Update documentation and presentation
</commit_message>
<xml_diff>
--- a/Documents/QA Documentation.xlsx
+++ b/Documents/QA Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirko\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-game\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19A41C21-8798-4748-B054-52D01D7D6ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0DFAB9-8D39-49B3-A35E-D8F23E72F25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17595" yWindow="4965" windowWidth="21600" windowHeight="11385" xr2:uid="{2D84E44C-68E2-40D3-88DA-E283613808FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{2D84E44C-68E2-40D3-88DA-E283613808FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,41 +304,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -348,11 +328,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -360,6 +336,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -679,7 +718,7 @@
   <dimension ref="B2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,366 +738,366 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="G5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="G6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="15" t="s">
+      <c r="G7" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="2">
+      <c r="C8" s="17">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="G8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="10" t="s">
+      <c r="G9" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="G10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="19">
+      <c r="C11" s="17">
         <v>3</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="5" t="s">
+      <c r="G11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="10" t="s">
+      <c r="G12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="13" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="15" t="s">
+      <c r="G13" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="19">
+      <c r="C14" s="17">
         <v>4</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="28" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="26" t="s">
+      <c r="G15" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="27" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="28" t="s">
+      <c r="G16" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="19">
+      <c r="C17" s="17">
         <v>5</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="28" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="35" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="26" t="s">
+      <c r="G18" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="27" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="28" t="s">
+      <c r="G19" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="33">
+      <c r="C20" s="22">
         <v>6</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="37" t="s">
+      <c r="G20" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="36" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>